<commit_message>
Remove data on Sep 28
</commit_message>
<xml_diff>
--- a/TMC/Total Tests by Date and Source.xlsx
+++ b/TMC/Total Tests by Date and Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yipenggao/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bpeng/ictr/covid-19-county-R0/TMC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A7FC5C1-6090-8643-BEA4-D760342F62B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74633320-8CA5-9540-B24A-E84B50B8B1B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8620" yWindow="1560" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total by Date - All Sources" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="231">
   <si>
     <t>Collected Date</t>
   </si>
@@ -1149,13 +1149,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D217"/>
+  <dimension ref="A1:D215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="A216" sqref="A216"/>
+    <sheetView tabSelected="1" topLeftCell="A210" zoomScale="249" zoomScaleNormal="249" workbookViewId="0">
+      <selection activeCell="A214" sqref="A214:XFD215"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -4145,46 +4145,20 @@
       </c>
     </row>
     <row r="214" spans="1:4" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A214" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B214" s="4">
-        <v>1</v>
-      </c>
-      <c r="C214" s="4">
-        <v>0</v>
-      </c>
-      <c r="D214" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A215" s="3"/>
-      <c r="B215" s="4">
-        <v>2822</v>
-      </c>
-      <c r="C215" s="4">
-        <v>356</v>
-      </c>
-      <c r="D215" s="4">
-        <v>3178</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A216" s="5" t="s">
+      <c r="A214" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="B216" s="6">
+      <c r="B214" s="6">
         <v>349882</v>
       </c>
-      <c r="C216" s="6">
+      <c r="C214" s="6">
         <v>43979</v>
       </c>
-      <c r="D216" s="6">
+      <c r="D214" s="6">
         <v>393861</v>
       </c>
     </row>
-    <row r="217" spans="1:4" s="1" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="215" spans="1:4" s="1" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -4198,7 +4172,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>

</xml_diff>